<commit_message>
this is the program for the compation
</commit_message>
<xml_diff>
--- a/MotorMappings.xlsx
+++ b/MotorMappings.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VexRobotics\turning-point-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A211605-C21C-41B0-9B52-E24D35086861}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F0B5DE-2A18-4D96-B3E6-2A39E352BDC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" activeTab="1" xr2:uid="{6F1AFA8A-84F4-4F21-A390-B07B212A9B34}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" activeTab="2" xr2:uid="{6F1AFA8A-84F4-4F21-A390-B07B212A9B34}"/>
   </bookViews>
   <sheets>
     <sheet name="1-5-19" sheetId="1" r:id="rId1"/>
     <sheet name="1-6-19" sheetId="3" r:id="rId2"/>
+    <sheet name="1-12-19" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
   <si>
     <t>rightLowerPlatformMotor</t>
   </si>
@@ -131,6 +132,21 @@
   </si>
   <si>
     <t>7u/7d</t>
+  </si>
+  <si>
+    <t>5U</t>
+  </si>
+  <si>
+    <t>6U</t>
+  </si>
+  <si>
+    <t>rubberMotor</t>
+  </si>
+  <si>
+    <t>8L</t>
+  </si>
+  <si>
+    <t>7L/7R</t>
   </si>
 </sst>
 </file>
@@ -631,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272368D6-111A-443F-B95C-88458551D513}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +696,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -688,7 +707,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
@@ -699,15 +721,159 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4583B334-0344-4D7A-8ED4-7F2B5EBFB163}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Motor Mappings based on new button placements
</commit_message>
<xml_diff>
--- a/MotorMappings.xlsx
+++ b/MotorMappings.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VexRobotics\turning-point-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F0B5DE-2A18-4D96-B3E6-2A39E352BDC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E1B633-E66A-496E-B8FA-6902CC4CEAB8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" activeTab="2" xr2:uid="{6F1AFA8A-84F4-4F21-A390-B07B212A9B34}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" activeTab="3" xr2:uid="{6F1AFA8A-84F4-4F21-A390-B07B212A9B34}"/>
   </bookViews>
   <sheets>
     <sheet name="1-5-19" sheetId="1" r:id="rId1"/>
     <sheet name="1-6-19" sheetId="3" r:id="rId2"/>
     <sheet name="1-12-19" sheetId="4" r:id="rId3"/>
+    <sheet name="1-17-19" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
   <si>
     <t>rightLowerPlatformMotor</t>
   </si>
@@ -147,6 +148,9 @@
   </si>
   <si>
     <t>7L/7R</t>
+  </si>
+  <si>
+    <t>7L</t>
   </si>
 </sst>
 </file>
@@ -785,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4583B334-0344-4D7A-8ED4-7F2B5EBFB163}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,4 +927,137 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041030D4-E3C4-4227-8A95-5F93FE5B5560}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>